<commit_message>
Getting to know parser
pseudo-Implemented <program> and <term> rules
</commit_message>
<xml_diff>
--- a/LL-table.xlsx
+++ b/LL-table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dokumnts\fiiit\IFJ\IFJ_2019_JJJJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{538EF9B5-4742-404A-A5CB-E54C59041463}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E96459-8D34-42EF-9A3A-C510566A6C1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8D276CB7-1AEA-4407-86D2-FC05F4DE124C}"/>
+    <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8964" xr2:uid="{8D276CB7-1AEA-4407-86D2-FC05F4DE124C}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -51,9 +51,6 @@
     <t>&lt;param_n&gt;</t>
   </si>
   <si>
-    <t>&lt;return&gt;</t>
-  </si>
-  <si>
     <t>&lt;return_value&gt;</t>
   </si>
   <si>
@@ -109,6 +106,9 @@
   </si>
   <si>
     <t>statement</t>
+  </si>
+  <si>
+    <t>&lt;statement_fun&gt;</t>
   </si>
 </sst>
 </file>
@@ -469,8 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7738B0FD-24E8-4698-88BB-BA79EA0966FE}">
   <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -481,49 +481,49 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
@@ -545,7 +545,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
@@ -573,7 +573,7 @@
         <v>8</v>
       </c>
       <c r="O5">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
@@ -602,67 +602,82 @@
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="G8">
-        <v>15</v>
+      <c r="H8">
+        <v>22</v>
       </c>
       <c r="O8">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>25</v>
+      </c>
+      <c r="D9">
+        <v>16</v>
+      </c>
+      <c r="G9">
+        <v>20</v>
       </c>
       <c r="H9">
+        <v>15</v>
+      </c>
+      <c r="I9">
         <v>17</v>
       </c>
+      <c r="J9">
+        <v>18</v>
+      </c>
+      <c r="K9">
+        <v>19</v>
+      </c>
       <c r="O9">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H10">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I10">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="J10">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="K10">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="O10">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M11">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="N11">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="H12">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Wrote most of my parts in documentation
</commit_message>
<xml_diff>
--- a/LL-table.xlsx
+++ b/LL-table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dokumnts\fiiit\IFJ\IFJ_2019_JJJJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E96459-8D34-42EF-9A3A-C510566A6C1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876D6199-A84E-4ECE-9A53-A9BFF0DAF6F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8964" xr2:uid="{8D276CB7-1AEA-4407-86D2-FC05F4DE124C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8D276CB7-1AEA-4407-86D2-FC05F4DE124C}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>&lt;program&gt;</t>
   </si>
@@ -103,9 +103,6 @@
   </si>
   <si>
     <t>EOF</t>
-  </si>
-  <si>
-    <t>statement</t>
   </si>
   <si>
     <t>&lt;statement_fun&gt;</t>
@@ -467,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7738B0FD-24E8-4698-88BB-BA79EA0966FE}">
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -479,7 +476,7 @@
     <col min="8" max="8" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>10</v>
       </c>
@@ -511,36 +508,45 @@
         <v>19</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="N1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
         <v>2</v>
       </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="P2">
+      <c r="D2">
+        <v>25</v>
+      </c>
+      <c r="H2">
+        <v>24</v>
+      </c>
+      <c r="I2">
+        <v>26</v>
+      </c>
+      <c r="J2">
+        <v>27</v>
+      </c>
+      <c r="K2">
+        <v>28</v>
+      </c>
+      <c r="O2">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -548,7 +554,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -561,57 +567,57 @@
       <c r="E4">
         <v>6</v>
       </c>
-      <c r="O4">
+      <c r="N4">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="F5">
         <v>8</v>
       </c>
-      <c r="O5">
+      <c r="N5">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="D6">
         <v>11</v>
       </c>
-      <c r="O6">
+      <c r="N6">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="F7">
         <v>13</v>
       </c>
-      <c r="O7">
+      <c r="N7">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="H8">
         <v>22</v>
       </c>
-      <c r="O8">
+      <c r="N8">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9">
         <v>16</v>
@@ -631,11 +637,11 @@
       <c r="K9">
         <v>19</v>
       </c>
-      <c r="O9">
+      <c r="N9">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -654,30 +660,33 @@
       <c r="K10">
         <v>28</v>
       </c>
-      <c r="O10">
+      <c r="N10">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
+      <c r="L11">
+        <v>30</v>
+      </c>
       <c r="M11">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N11">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
       <c r="D12">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H12">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>